<commit_message>
Elimine las piezas grandes con dos procesos largos
</commit_message>
<xml_diff>
--- a/datos_reordenados/archivo_reordenado.xlsx
+++ b/datos_reordenados/archivo_reordenado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,22 +497,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>98231</v>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="n">
-        <v>5.739389999999999</v>
-      </c>
+        <v>94105</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.566335</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>5.73939</v>
+        <v>1.566335</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -521,7 +521,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>2</v>
@@ -529,20 +529,20 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>26401</v>
-      </c>
-      <c r="B3" t="n">
-        <v>6.317955</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
+        <v>39570</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>1.9446</v>
+      </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>6.317955</v>
+        <v>1.9446</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -551,7 +551,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3" t="n">
         <v>2</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>51523</v>
+        <v>15821</v>
       </c>
       <c r="B4" t="n">
         <v>8.2979</v>
@@ -591,20 +591,20 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>28232</v>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="n">
-        <v>2.9125</v>
-      </c>
+        <v>26401</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6.317955</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>2.9125</v>
+        <v>6.317955</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
         <v>2</v>
@@ -621,28 +621,26 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>29419</v>
+        <v>28232</v>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>9.29157</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
+        <v>2.9125</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
         <v>2</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>9.29157</v>
+        <v>2.9125</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
         <v>2</v>
@@ -653,32 +651,38 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>55629</v>
+        <v>54881</v>
       </c>
       <c r="B7" t="n">
-        <v>3.4675</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+        <v>6.912355</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>1</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
       <c r="H7" t="n">
-        <v>3.4675</v>
+        <v>12.702355</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -713,29 +717,31 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>66872</v>
-      </c>
-      <c r="B9" t="n">
-        <v>4.82843</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+        <v>35038</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>7.7179</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>4.82843</v>
+        <v>7.7179</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" t="n">
         <v>2</v>
@@ -743,31 +749,29 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>94105</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1.566335</v>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
+        <v>56513</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>3.8271</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>1.566335</v>
+        <v>3.8271</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L10" t="n">
         <v>2</v>
@@ -775,11 +779,11 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>56513</v>
+        <v>83362</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>3.8271</v>
+        <v>2.96212</v>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -788,7 +792,7 @@
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
-        <v>3.8271</v>
+        <v>2.96212</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -805,62 +809,56 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>80150</v>
+        <v>66872</v>
       </c>
       <c r="B12" t="n">
-        <v>8.8797</v>
-      </c>
-      <c r="C12" t="n">
-        <v>7.5849</v>
-      </c>
+        <v>4.82843</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
         <v>1</v>
       </c>
-      <c r="G12" t="n">
-        <v>2</v>
-      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>16.4646</v>
+        <v>4.82843</v>
       </c>
       <c r="I12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>18234</v>
+        <v>84035</v>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="n">
-        <v>2.9125</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
+        <v>6.6362</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>2</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
-        <v>2.9125</v>
+        <v>6.6362</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>2</v>
@@ -871,20 +869,20 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12569</v>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="n">
-        <v>14.712495</v>
-      </c>
+        <v>62510</v>
+      </c>
+      <c r="B14" t="n">
+        <v>8.7338</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
-        <v>14.712495</v>
+        <v>8.7338</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
@@ -893,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14" t="n">
         <v>2</v>
@@ -901,31 +899,29 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>48436</v>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="n">
-        <v>7.7179</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
+        <v>85551</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5.48275</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>7.7179</v>
+        <v>5.48275</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
@@ -933,20 +929,20 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>39570</v>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="n">
-        <v>1.9446</v>
-      </c>
+        <v>86806</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5.175845</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
-        <v>1.9446</v>
+        <v>5.175845</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>
@@ -955,7 +951,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
         <v>2</v>
@@ -963,22 +959,22 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>41846</v>
-      </c>
-      <c r="B17" t="n">
-        <v>32.67480999999999</v>
-      </c>
-      <c r="C17" t="inlineStr"/>
+        <v>37026</v>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="n">
+        <v>8.113350000000001</v>
+      </c>
       <c r="D17" t="n">
         <v>1</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>32.67481</v>
+        <v>8.113350000000001</v>
       </c>
       <c r="I17" t="n">
         <v>1</v>
@@ -987,7 +983,7 @@
         <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" t="n">
         <v>2</v>
@@ -995,93 +991,95 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>78875</v>
+        <v>58964</v>
       </c>
       <c r="B18" t="n">
-        <v>2.128375</v>
-      </c>
-      <c r="C18" t="inlineStr"/>
+        <v>11.119145</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9.324244999999999</v>
+      </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
         <v>1</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>2</v>
+      </c>
       <c r="H18" t="n">
-        <v>2.128375</v>
+        <v>20.44339</v>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>94963</v>
+        <v>68056</v>
       </c>
       <c r="B19" t="n">
-        <v>11.119145</v>
-      </c>
-      <c r="C19" t="n">
-        <v>9.324244999999999</v>
-      </c>
+        <v>26.826</v>
+      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
         <v>1</v>
       </c>
-      <c r="G19" t="n">
-        <v>2</v>
-      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
-        <v>20.44339</v>
+        <v>26.826</v>
       </c>
       <c r="I19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>68056</v>
-      </c>
-      <c r="B20" t="n">
-        <v>26.826</v>
-      </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+        <v>54637</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>6.89765</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
-        <v>26.826</v>
+        <v>6.89765</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L20" t="n">
         <v>2</v>
@@ -1089,22 +1087,22 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>22941</v>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="n">
-        <v>9.61735</v>
-      </c>
+        <v>80744</v>
+      </c>
+      <c r="B21" t="n">
+        <v>17.531</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>1</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>9.61735</v>
+        <v>17.531</v>
       </c>
       <c r="I21" t="n">
         <v>1</v>
@@ -1113,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L21" t="n">
         <v>2</v>
@@ -1121,10 +1119,10 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>62510</v>
+        <v>39977</v>
       </c>
       <c r="B22" t="n">
-        <v>8.7338</v>
+        <v>1.8118</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
@@ -1134,7 +1132,7 @@
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
-        <v>8.7338</v>
+        <v>1.8118</v>
       </c>
       <c r="I22" t="n">
         <v>1</v>
@@ -1151,54 +1149,52 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>15166</v>
-      </c>
-      <c r="B23" t="n">
-        <v>2.39973</v>
-      </c>
+        <v>29419</v>
+      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="n">
-        <v>4.48595</v>
-      </c>
-      <c r="D23" t="inlineStr"/>
+        <v>9.29157</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
-        <v>6.88568</v>
+        <v>9.29157</v>
       </c>
       <c r="I23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="n">
         <v>2</v>
       </c>
       <c r="L23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>86806</v>
-      </c>
-      <c r="B24" t="n">
-        <v>5.175845</v>
-      </c>
-      <c r="C24" t="inlineStr"/>
+        <v>16739</v>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>6.6362</v>
+      </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>5.175845</v>
+        <v>6.6362</v>
       </c>
       <c r="I24" t="n">
         <v>1</v>
@@ -1207,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L24" t="n">
         <v>2</v>
@@ -1215,61 +1211,65 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>62448</v>
-      </c>
-      <c r="B25" t="inlineStr"/>
+        <v>80150</v>
+      </c>
+      <c r="B25" t="n">
+        <v>8.8797</v>
+      </c>
       <c r="C25" t="n">
-        <v>1.9446</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1</v>
-      </c>
+        <v>7.5849</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>2</v>
-      </c>
-      <c r="G25" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2</v>
+      </c>
       <c r="H25" t="n">
-        <v>1.9446</v>
+        <v>16.4646</v>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
         <v>2</v>
       </c>
       <c r="L25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>84035</v>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="n">
-        <v>6.6362</v>
-      </c>
-      <c r="D26" t="inlineStr"/>
+        <v>86468</v>
+      </c>
+      <c r="B26" t="n">
+        <v>9.42925</v>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>6.6362</v>
+        <v>9.42925</v>
       </c>
       <c r="I26" t="n">
         <v>1</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L26" t="n">
         <v>2</v>
@@ -1277,24 +1277,24 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>58964</v>
+        <v>98208</v>
       </c>
       <c r="B27" t="n">
-        <v>11.119145</v>
+        <v>16.1256</v>
       </c>
       <c r="C27" t="n">
-        <v>9.324244999999999</v>
+        <v>4.55664</v>
       </c>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" t="n">
-        <v>20.44339</v>
+        <v>20.68224</v>
       </c>
       <c r="I27" t="n">
         <v>2</v>
@@ -1303,73 +1303,73 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>15243</v>
+        <v>94963</v>
       </c>
       <c r="B28" t="n">
-        <v>19.733855</v>
+        <v>11.119145</v>
       </c>
       <c r="C28" t="n">
-        <v>8.911380000000001</v>
-      </c>
-      <c r="D28" t="n">
-        <v>1</v>
-      </c>
+        <v>9.324244999999999</v>
+      </c>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" t="n">
-        <v>28.645235</v>
+        <v>20.44339</v>
       </c>
       <c r="I28" t="n">
         <v>2</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>30555</v>
-      </c>
-      <c r="B29" t="n">
-        <v>26.826</v>
-      </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+        <v>62448</v>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="n">
+        <v>1.9446</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
-        <v>26.826</v>
+        <v>1.9446</v>
       </c>
       <c r="I29" t="n">
         <v>1</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L29" t="n">
         <v>2</v>
@@ -1377,13 +1377,11 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>92317</v>
-      </c>
-      <c r="B30" t="n">
-        <v>5.1623</v>
-      </c>
+        <v>18234</v>
+      </c>
+      <c r="B30" t="inlineStr"/>
       <c r="C30" t="n">
-        <v>3.1675</v>
+        <v>2.9125</v>
       </c>
       <c r="D30" t="n">
         <v>1</v>
@@ -1392,20 +1390,18 @@
       <c r="F30" t="n">
         <v>2</v>
       </c>
-      <c r="G30" t="n">
-        <v>1</v>
-      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
-        <v>8.329800000000001</v>
+        <v>2.9125</v>
       </c>
       <c r="I30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J30" t="n">
         <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L30" t="n">
         <v>2</v>
@@ -1413,31 +1409,29 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>36940</v>
-      </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="n">
-        <v>9.61735</v>
-      </c>
-      <c r="D31" t="n">
-        <v>1</v>
-      </c>
+        <v>23953</v>
+      </c>
+      <c r="B31" t="n">
+        <v>26.5956</v>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>9.61735</v>
+        <v>26.5956</v>
       </c>
       <c r="I31" t="n">
         <v>1</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L31" t="n">
         <v>2</v>
@@ -1445,10 +1439,10 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>58257</v>
+        <v>30555</v>
       </c>
       <c r="B32" t="n">
-        <v>2.76655</v>
+        <v>26.826</v>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
@@ -1458,7 +1452,7 @@
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
-        <v>2.76655</v>
+        <v>26.826</v>
       </c>
       <c r="I32" t="n">
         <v>1</v>
@@ -1475,29 +1469,25 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>54881</v>
-      </c>
-      <c r="B33" t="n">
-        <v>6.912355</v>
-      </c>
+        <v>30122</v>
+      </c>
+      <c r="B33" t="inlineStr"/>
       <c r="C33" t="n">
-        <v>5.79</v>
+        <v>3.39928</v>
       </c>
       <c r="D33" t="n">
         <v>1</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
-        <v>12.702355</v>
+        <v>3.39928</v>
       </c>
       <c r="I33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" t="n">
         <v>1</v>
@@ -1506,29 +1496,29 @@
         <v>2</v>
       </c>
       <c r="L33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>98208</v>
+        <v>15166</v>
       </c>
       <c r="B34" t="n">
-        <v>16.1256</v>
+        <v>2.39973</v>
       </c>
       <c r="C34" t="n">
-        <v>4.55664</v>
+        <v>4.48595</v>
       </c>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H34" t="n">
-        <v>20.68224</v>
+        <v>6.88568</v>
       </c>
       <c r="I34" t="n">
         <v>2</v>
@@ -1537,18 +1527,18 @@
         <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>85551</v>
+        <v>55629</v>
       </c>
       <c r="B35" t="n">
-        <v>5.48275</v>
+        <v>3.4675</v>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
@@ -1558,7 +1548,7 @@
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>5.48275</v>
+        <v>3.4675</v>
       </c>
       <c r="I35" t="n">
         <v>1</v>
@@ -1575,26 +1565,28 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>51554</v>
+        <v>88645</v>
       </c>
       <c r="B36" t="n">
-        <v>28.8416</v>
+        <v>32.67480999999999</v>
       </c>
       <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
         <v>1</v>
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>28.8416</v>
+        <v>32.67480999999999</v>
       </c>
       <c r="I36" t="n">
         <v>1</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" t="n">
         <v>1</v>
@@ -1605,11 +1597,11 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>90820</v>
+        <v>78414</v>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="n">
-        <v>8.113350000000001</v>
+        <v>9.13414</v>
       </c>
       <c r="D37" t="n">
         <v>1</v>
@@ -1620,7 +1612,7 @@
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
-        <v>8.113350000000001</v>
+        <v>9.13414</v>
       </c>
       <c r="I37" t="n">
         <v>1</v>
@@ -1637,31 +1629,29 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>86468</v>
-      </c>
-      <c r="B38" t="n">
-        <v>9.42925</v>
-      </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="n">
-        <v>1</v>
-      </c>
+        <v>14559</v>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="n">
+        <v>0.97684</v>
+      </c>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
-        <v>9.42925</v>
+        <v>0.97684</v>
       </c>
       <c r="I38" t="n">
         <v>1</v>
       </c>
       <c r="J38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L38" t="n">
         <v>2</v>
@@ -1669,31 +1659,29 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>37026</v>
-      </c>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="n">
-        <v>8.113350000000001</v>
-      </c>
-      <c r="D39" t="n">
-        <v>1</v>
-      </c>
+        <v>27704</v>
+      </c>
+      <c r="B39" t="n">
+        <v>6.3156</v>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
-        <v>8.113350000000001</v>
+        <v>6.3156</v>
       </c>
       <c r="I39" t="n">
         <v>1</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L39" t="n">
         <v>2</v>
@@ -1701,22 +1689,22 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>88645</v>
-      </c>
-      <c r="B40" t="n">
-        <v>32.67480999999999</v>
-      </c>
-      <c r="C40" t="inlineStr"/>
+        <v>90820</v>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="n">
+        <v>8.113350000000001</v>
+      </c>
       <c r="D40" t="n">
         <v>1</v>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
-        <v>32.67481</v>
+        <v>8.113350000000001</v>
       </c>
       <c r="I40" t="n">
         <v>1</v>
@@ -1725,7 +1713,7 @@
         <v>1</v>
       </c>
       <c r="K40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L40" t="n">
         <v>2</v>
@@ -1733,11 +1721,11 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>78414</v>
+        <v>53842</v>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="n">
-        <v>9.13414</v>
+        <v>6.89765</v>
       </c>
       <c r="D41" t="n">
         <v>1</v>
@@ -1748,7 +1736,7 @@
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
-        <v>9.13414</v>
+        <v>6.89765</v>
       </c>
       <c r="I41" t="n">
         <v>1</v>
@@ -1765,23 +1753,27 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>39977</v>
+        <v>71809</v>
       </c>
       <c r="B42" t="n">
-        <v>1.8118</v>
-      </c>
-      <c r="C42" t="inlineStr"/>
+        <v>16.1256</v>
+      </c>
+      <c r="C42" t="n">
+        <v>4.55664</v>
+      </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1</v>
+      </c>
       <c r="H42" t="n">
-        <v>1.8118</v>
+        <v>20.68224</v>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J42" t="n">
         <v>0</v>
@@ -1795,20 +1787,20 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>27704</v>
-      </c>
-      <c r="B43" t="n">
-        <v>6.3156</v>
-      </c>
-      <c r="C43" t="inlineStr"/>
+        <v>49265</v>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="n">
+        <v>7.747554999999999</v>
+      </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
-        <v>6.3156</v>
+        <v>7.747554999999999</v>
       </c>
       <c r="I43" t="n">
         <v>1</v>
@@ -1817,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="K43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L43" t="n">
         <v>2</v>
@@ -1825,31 +1817,29 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>61318</v>
-      </c>
-      <c r="B44" t="n">
-        <v>33.3234</v>
-      </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="n">
-        <v>1</v>
-      </c>
+        <v>63907</v>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="n">
+        <v>2.16215</v>
+      </c>
+      <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>33.3234</v>
+        <v>2.16215</v>
       </c>
       <c r="I44" t="n">
         <v>1</v>
       </c>
       <c r="J44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L44" t="n">
         <v>2</v>
@@ -1857,26 +1847,28 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>16739</v>
+        <v>36940</v>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="n">
-        <v>6.6362</v>
-      </c>
-      <c r="D45" t="inlineStr"/>
+        <v>9.61735</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="n">
         <v>2</v>
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>6.6362</v>
+        <v>9.61735</v>
       </c>
       <c r="I45" t="n">
         <v>1</v>
       </c>
       <c r="J45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" t="n">
         <v>2</v>
@@ -1887,13 +1879,13 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>71809</v>
+        <v>63574</v>
       </c>
       <c r="B46" t="n">
-        <v>16.1256</v>
+        <v>1.57876</v>
       </c>
       <c r="C46" t="n">
-        <v>4.55664</v>
+        <v>15.547135</v>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
@@ -1904,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="H46" t="n">
-        <v>20.68224</v>
+        <v>17.125895</v>
       </c>
       <c r="I46" t="n">
         <v>2</v>
@@ -1921,28 +1913,30 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>58167</v>
+        <v>18960</v>
       </c>
       <c r="B47" t="n">
-        <v>14.928885</v>
-      </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="n">
-        <v>1</v>
-      </c>
+        <v>1.88945</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.76964</v>
+      </c>
+      <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G47" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1</v>
+      </c>
       <c r="H47" t="n">
-        <v>14.928885</v>
+        <v>2.65909</v>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" t="n">
         <v>1</v>
@@ -1953,20 +1947,20 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>63907</v>
-      </c>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="n">
-        <v>2.16215</v>
-      </c>
+        <v>23852</v>
+      </c>
+      <c r="B48" t="n">
+        <v>24.64169</v>
+      </c>
+      <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
-        <v>2.16215</v>
+        <v>24.64169</v>
       </c>
       <c r="I48" t="n">
         <v>1</v>
@@ -1975,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L48" t="n">
         <v>2</v>
@@ -1983,25 +1977,29 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>54637</v>
-      </c>
-      <c r="B49" t="inlineStr"/>
+        <v>16680</v>
+      </c>
+      <c r="B49" t="n">
+        <v>6.912355</v>
+      </c>
       <c r="C49" t="n">
-        <v>6.89765</v>
+        <v>5.79</v>
       </c>
       <c r="D49" t="n">
         <v>1</v>
       </c>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="n">
-        <v>2</v>
-      </c>
-      <c r="G49" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="G49" t="n">
+        <v>2</v>
+      </c>
       <c r="H49" t="n">
-        <v>6.89765</v>
+        <v>12.702355</v>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J49" t="n">
         <v>1</v>
@@ -2010,35 +2008,33 @@
         <v>2</v>
       </c>
       <c r="L49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>63574</v>
+        <v>61318</v>
       </c>
       <c r="B50" t="n">
-        <v>1.57876</v>
-      </c>
-      <c r="C50" t="n">
-        <v>15.547135</v>
-      </c>
-      <c r="D50" t="inlineStr"/>
+        <v>33.3234</v>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="n">
-        <v>2</v>
-      </c>
-      <c r="G50" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>17.125895</v>
+        <v>33.3234</v>
       </c>
       <c r="I50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" t="n">
         <v>1</v>
@@ -2049,26 +2045,28 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>14559</v>
+        <v>98231</v>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="n">
-        <v>0.97684</v>
-      </c>
-      <c r="D51" t="inlineStr"/>
+        <v>5.739389999999999</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="n">
         <v>2</v>
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
-        <v>0.97684</v>
+        <v>5.739389999999999</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
       </c>
       <c r="J51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" t="n">
         <v>2</v>
@@ -2079,29 +2077,25 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>38047</v>
+        <v>41846</v>
       </c>
       <c r="B52" t="n">
-        <v>5.122635</v>
-      </c>
-      <c r="C52" t="n">
-        <v>1.57645</v>
-      </c>
+        <v>32.67480999999999</v>
+      </c>
+      <c r="C52" t="inlineStr"/>
       <c r="D52" t="n">
         <v>1</v>
       </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="n">
-        <v>2</v>
-      </c>
-      <c r="G52" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G52" t="inlineStr"/>
       <c r="H52" t="n">
-        <v>6.699085</v>
+        <v>32.67480999999999</v>
       </c>
       <c r="I52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J52" t="n">
         <v>1</v>
@@ -2115,68 +2109,56 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>16680</v>
-      </c>
-      <c r="B53" t="n">
-        <v>6.912355</v>
-      </c>
+        <v>76530</v>
+      </c>
+      <c r="B53" t="inlineStr"/>
       <c r="C53" t="n">
-        <v>5.79</v>
-      </c>
-      <c r="D53" t="n">
-        <v>1</v>
-      </c>
+        <v>2.745975</v>
+      </c>
+      <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="n">
-        <v>1</v>
-      </c>
-      <c r="G53" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
-        <v>12.702355</v>
+        <v>2.745975</v>
       </c>
       <c r="I53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53" t="n">
         <v>2</v>
       </c>
       <c r="L53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>19816</v>
+        <v>51554</v>
       </c>
       <c r="B54" t="n">
-        <v>5.1623</v>
-      </c>
-      <c r="C54" t="n">
-        <v>3.1675</v>
-      </c>
-      <c r="D54" t="n">
-        <v>1</v>
-      </c>
+        <v>28.8416</v>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="n">
-        <v>2</v>
-      </c>
-      <c r="G54" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
-        <v>8.329800000000001</v>
+        <v>28.8416</v>
       </c>
       <c r="I54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K54" t="n">
         <v>1</v>
@@ -2219,28 +2201,26 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>53842</v>
+        <v>12569</v>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="n">
-        <v>6.89765</v>
-      </c>
-      <c r="D56" t="n">
-        <v>1</v>
-      </c>
+        <v>14.712495</v>
+      </c>
+      <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="n">
         <v>2</v>
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
-        <v>6.89765</v>
+        <v>14.712495</v>
       </c>
       <c r="I56" t="n">
         <v>1</v>
       </c>
       <c r="J56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56" t="n">
         <v>2</v>
@@ -2251,28 +2231,26 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>20627</v>
+        <v>98173</v>
       </c>
       <c r="B57" t="n">
-        <v>33.3234</v>
+        <v>4.56445</v>
       </c>
       <c r="C57" t="inlineStr"/>
-      <c r="D57" t="n">
-        <v>1</v>
-      </c>
+      <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="n">
         <v>1</v>
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="n">
-        <v>33.3234</v>
+        <v>4.56445</v>
       </c>
       <c r="I57" t="n">
         <v>1</v>
       </c>
       <c r="J57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57" t="n">
         <v>1</v>
@@ -2283,20 +2261,20 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>39749</v>
-      </c>
-      <c r="B58" t="n">
-        <v>2.128375</v>
-      </c>
-      <c r="C58" t="inlineStr"/>
+        <v>21512</v>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="n">
+        <v>3.8271</v>
+      </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
-        <v>2.128375</v>
+        <v>3.8271</v>
       </c>
       <c r="I58" t="n">
         <v>1</v>
@@ -2305,7 +2283,7 @@
         <v>0</v>
       </c>
       <c r="K58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L58" t="n">
         <v>2</v>
@@ -2313,11 +2291,11 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>61625</v>
+        <v>48436</v>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="n">
-        <v>5.21835</v>
+        <v>7.7179</v>
       </c>
       <c r="D59" t="n">
         <v>1</v>
@@ -2328,7 +2306,7 @@
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
-        <v>5.21835</v>
+        <v>7.7179</v>
       </c>
       <c r="I59" t="n">
         <v>1</v>
@@ -2345,28 +2323,26 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>80744</v>
+        <v>96876</v>
       </c>
       <c r="B60" t="n">
-        <v>17.531</v>
+        <v>0.93293</v>
       </c>
       <c r="C60" t="inlineStr"/>
-      <c r="D60" t="n">
-        <v>1</v>
-      </c>
+      <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="n">
         <v>1</v>
       </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
-        <v>17.531</v>
+        <v>0.93293</v>
       </c>
       <c r="I60" t="n">
         <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" t="n">
         <v>1</v>
@@ -2377,10 +2353,10 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>78578</v>
+        <v>64371</v>
       </c>
       <c r="B61" t="n">
-        <v>1.8118</v>
+        <v>8.752000000000001</v>
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
@@ -2390,7 +2366,7 @@
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
-        <v>1.8118</v>
+        <v>8.752000000000001</v>
       </c>
       <c r="I61" t="n">
         <v>1</v>
@@ -2407,29 +2383,31 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>46858</v>
-      </c>
-      <c r="B62" t="n">
-        <v>26.5956</v>
-      </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+        <v>22941</v>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="n">
+        <v>9.61735</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
-        <v>26.5956</v>
+        <v>9.61735</v>
       </c>
       <c r="I62" t="n">
         <v>1</v>
       </c>
       <c r="J62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L62" t="n">
         <v>2</v>
@@ -2437,11 +2415,11 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>21512</v>
+        <v>61633</v>
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="n">
-        <v>3.8271</v>
+        <v>2.745975</v>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
@@ -2450,7 +2428,7 @@
       </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="n">
-        <v>3.8271</v>
+        <v>2.745975</v>
       </c>
       <c r="I63" t="n">
         <v>1</v>
@@ -2467,20 +2445,20 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>61633</v>
-      </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="n">
-        <v>2.745975</v>
-      </c>
+        <v>39749</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2.128375</v>
+      </c>
+      <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
-        <v>2.745975</v>
+        <v>2.128375</v>
       </c>
       <c r="I64" t="n">
         <v>1</v>
@@ -2489,7 +2467,7 @@
         <v>0</v>
       </c>
       <c r="K64" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L64" t="n">
         <v>2</v>
@@ -2497,10 +2475,10 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>96876</v>
+        <v>78875</v>
       </c>
       <c r="B65" t="n">
-        <v>0.93293</v>
+        <v>2.128375</v>
       </c>
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr"/>
@@ -2510,7 +2488,7 @@
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
-        <v>0.93293</v>
+        <v>2.128375</v>
       </c>
       <c r="I65" t="n">
         <v>1</v>
@@ -2527,27 +2505,23 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>18960</v>
+        <v>91802</v>
       </c>
       <c r="B66" t="n">
-        <v>1.88945</v>
-      </c>
-      <c r="C66" t="n">
-        <v>0.76964</v>
-      </c>
+        <v>6.3156</v>
+      </c>
+      <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="n">
-        <v>2</v>
-      </c>
-      <c r="G66" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
-        <v>2.65909</v>
+        <v>6.3156</v>
       </c>
       <c r="I66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J66" t="n">
         <v>0</v>
@@ -2561,20 +2535,20 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>49265</v>
-      </c>
-      <c r="B67" t="inlineStr"/>
-      <c r="C67" t="n">
-        <v>7.747554999999999</v>
-      </c>
+        <v>46858</v>
+      </c>
+      <c r="B67" t="n">
+        <v>26.5956</v>
+      </c>
+      <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="n">
-        <v>7.747555</v>
+        <v>26.5956</v>
       </c>
       <c r="I67" t="n">
         <v>1</v>
@@ -2583,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="K67" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L67" t="n">
         <v>2</v>
@@ -2591,29 +2565,31 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>64371</v>
-      </c>
-      <c r="B68" t="n">
-        <v>8.752000000000001</v>
-      </c>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
+        <v>61625</v>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="n">
+        <v>5.21835</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="n">
-        <v>8.752000000000001</v>
+        <v>5.21835</v>
       </c>
       <c r="I68" t="n">
         <v>1</v>
       </c>
       <c r="J68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L68" t="n">
         <v>2</v>
@@ -2621,31 +2597,29 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>35038</v>
-      </c>
-      <c r="B69" t="inlineStr"/>
-      <c r="C69" t="n">
-        <v>7.7179</v>
-      </c>
-      <c r="D69" t="n">
-        <v>1</v>
-      </c>
+        <v>48903</v>
+      </c>
+      <c r="B69" t="n">
+        <v>6.3156</v>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
-        <v>7.7179</v>
+        <v>6.3156</v>
       </c>
       <c r="I69" t="n">
         <v>1</v>
       </c>
       <c r="J69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L69" t="n">
         <v>2</v>
@@ -2653,29 +2627,31 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>76530</v>
-      </c>
-      <c r="B70" t="inlineStr"/>
-      <c r="C70" t="n">
-        <v>2.745975</v>
-      </c>
-      <c r="D70" t="inlineStr"/>
+        <v>20627</v>
+      </c>
+      <c r="B70" t="n">
+        <v>33.3234</v>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="n">
-        <v>2.745975</v>
+        <v>33.3234</v>
       </c>
       <c r="I70" t="n">
         <v>1</v>
       </c>
       <c r="J70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L70" t="n">
         <v>2</v>
@@ -2683,26 +2659,28 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>91802</v>
+        <v>51523</v>
       </c>
       <c r="B71" t="n">
-        <v>6.3156</v>
+        <v>8.2979</v>
       </c>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="n">
         <v>1</v>
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
-        <v>6.3156</v>
+        <v>8.2979</v>
       </c>
       <c r="I71" t="n">
         <v>1</v>
       </c>
       <c r="J71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K71" t="n">
         <v>1</v>
@@ -2713,26 +2691,28 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>23953</v>
+        <v>58167</v>
       </c>
       <c r="B72" t="n">
-        <v>26.5956</v>
+        <v>14.928885</v>
       </c>
       <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="n">
         <v>1</v>
       </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="n">
-        <v>26.5956</v>
+        <v>14.928885</v>
       </c>
       <c r="I72" t="n">
         <v>1</v>
       </c>
       <c r="J72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K72" t="n">
         <v>1</v>
@@ -2743,31 +2723,29 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>30122</v>
-      </c>
-      <c r="B73" t="inlineStr"/>
-      <c r="C73" t="n">
-        <v>3.39928</v>
-      </c>
-      <c r="D73" t="n">
-        <v>1</v>
-      </c>
+        <v>78578</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1.8118</v>
+      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="n">
-        <v>3.39928</v>
+        <v>1.8118</v>
       </c>
       <c r="I73" t="n">
         <v>1</v>
       </c>
       <c r="J73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L73" t="n">
         <v>2</v>
@@ -2775,29 +2753,31 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>48903</v>
-      </c>
-      <c r="B74" t="n">
-        <v>6.3156</v>
-      </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
+        <v>40815</v>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="n">
+        <v>9.13414</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="n">
-        <v>6.3156</v>
+        <v>9.13414</v>
       </c>
       <c r="I74" t="n">
         <v>1</v>
       </c>
       <c r="J74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L74" t="n">
         <v>2</v>
@@ -2805,191 +2785,31 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>43524</v>
+        <v>58257</v>
       </c>
       <c r="B75" t="n">
-        <v>8.32</v>
-      </c>
-      <c r="C75" t="n">
-        <v>8.599219999999999</v>
-      </c>
-      <c r="D75" t="n">
-        <v>1</v>
-      </c>
+        <v>2.76655</v>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="n">
-        <v>2</v>
-      </c>
-      <c r="G75" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
-        <v>16.91922</v>
+        <v>2.76655</v>
       </c>
       <c r="I75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K75" t="n">
         <v>1</v>
       </c>
       <c r="L75" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>15821</v>
-      </c>
-      <c r="B76" t="n">
-        <v>8.2979</v>
-      </c>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="n">
-        <v>1</v>
-      </c>
-      <c r="E76" t="inlineStr"/>
-      <c r="F76" t="n">
-        <v>1</v>
-      </c>
-      <c r="G76" t="inlineStr"/>
-      <c r="H76" t="n">
-        <v>8.2979</v>
-      </c>
-      <c r="I76" t="n">
-        <v>1</v>
-      </c>
-      <c r="J76" t="n">
-        <v>1</v>
-      </c>
-      <c r="K76" t="n">
-        <v>1</v>
-      </c>
-      <c r="L76" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>83362</v>
-      </c>
-      <c r="B77" t="inlineStr"/>
-      <c r="C77" t="n">
-        <v>2.96212</v>
-      </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
-      <c r="F77" t="n">
-        <v>2</v>
-      </c>
-      <c r="G77" t="inlineStr"/>
-      <c r="H77" t="n">
-        <v>2.96212</v>
-      </c>
-      <c r="I77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J77" t="n">
-        <v>0</v>
-      </c>
-      <c r="K77" t="n">
-        <v>2</v>
-      </c>
-      <c r="L77" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>98173</v>
-      </c>
-      <c r="B78" t="n">
-        <v>4.56445</v>
-      </c>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
-      <c r="F78" t="n">
-        <v>1</v>
-      </c>
-      <c r="G78" t="inlineStr"/>
-      <c r="H78" t="n">
-        <v>4.56445</v>
-      </c>
-      <c r="I78" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" t="n">
-        <v>0</v>
-      </c>
-      <c r="K78" t="n">
-        <v>1</v>
-      </c>
-      <c r="L78" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>40815</v>
-      </c>
-      <c r="B79" t="inlineStr"/>
-      <c r="C79" t="n">
-        <v>9.13414</v>
-      </c>
-      <c r="D79" t="n">
-        <v>1</v>
-      </c>
-      <c r="E79" t="inlineStr"/>
-      <c r="F79" t="n">
-        <v>2</v>
-      </c>
-      <c r="G79" t="inlineStr"/>
-      <c r="H79" t="n">
-        <v>9.13414</v>
-      </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="n">
-        <v>1</v>
-      </c>
-      <c r="K79" t="n">
-        <v>2</v>
-      </c>
-      <c r="L79" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>23852</v>
-      </c>
-      <c r="B80" t="n">
-        <v>24.64169</v>
-      </c>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
-      <c r="F80" t="n">
-        <v>1</v>
-      </c>
-      <c r="G80" t="inlineStr"/>
-      <c r="H80" t="n">
-        <v>24.64169</v>
-      </c>
-      <c r="I80" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" t="n">
-        <v>0</v>
-      </c>
-      <c r="K80" t="n">
-        <v>1</v>
-      </c>
-      <c r="L80" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>